<commit_message>
Remove QR Code Generator functionality and related code
</commit_message>
<xml_diff>
--- a/Gate Pass & Issuance/Gate pass.xlsx
+++ b/Gate Pass & Issuance/Gate pass.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gate Pass &amp; Issuance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding Projects\eminventorysystem\Gate Pass &amp; Issuance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D70F0DB-1A12-415B-A497-E0DE281F9FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B05E1FC-6A18-4328-B204-B6D98FD1111C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,22 +19,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tools issuance slip'!$A$1:$K$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>E &amp; M Sub-Department</t>
   </si>
@@ -78,46 +67,19 @@
     <t>To be filled by receiver:</t>
   </si>
   <si>
-    <t>Department: E&amp;M Systems</t>
-  </si>
-  <si>
     <t>Gate Pass</t>
   </si>
   <si>
-    <t>Designation: E&amp;M Systems Technician</t>
+    <t>Issuer Name:</t>
   </si>
   <si>
-    <t>Nos</t>
+    <t>Contact:</t>
   </si>
   <si>
-    <t>Date:      09-04-2025</t>
+    <t>Designation:</t>
   </si>
   <si>
-    <t>Rainwater Motor</t>
-  </si>
-  <si>
-    <t>Soft Starter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zohaib </t>
-  </si>
-  <si>
-    <t>EPC-Dept-1</t>
-  </si>
-  <si>
-    <t>Waqar Younas</t>
-  </si>
-  <si>
-    <t>0342-4528216</t>
-  </si>
-  <si>
-    <t>Issuer Name: Faizan Ali</t>
-  </si>
-  <si>
-    <t>Contact: 0303-5212027</t>
-  </si>
-  <si>
-    <t>OLT NO. 1604</t>
+    <t>Date:</t>
   </si>
 </sst>
 </file>
@@ -700,10 +662,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -712,16 +698,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
@@ -738,117 +811,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1467,8 +1429,8 @@
   </sheetPr>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:K9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48:K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1481,637 +1443,625 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="51"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="50"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="52"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="54"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="59"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A5" s="60"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="62"/>
+    </row>
+    <row r="6" spans="1:11" ht="19.899999999999999" customHeight="1">
+      <c r="A6" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="60"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A5" s="61"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="63"/>
-    </row>
-    <row r="6" spans="1:11" ht="19.899999999999999" customHeight="1">
-      <c r="A6" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="64" t="s">
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="68"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="67"/>
     </row>
     <row r="7" spans="1:11" ht="19.899999999999999" customHeight="1">
-      <c r="A7" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="40" t="s">
+      <c r="A7" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="41"/>
+    </row>
+    <row r="8" spans="1:11" ht="19.899999999999999" customHeight="1">
+      <c r="A8" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="42"/>
-    </row>
-    <row r="8" spans="1:11" ht="19.899999999999999" customHeight="1">
-      <c r="A8" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="43" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="45"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="44"/>
     </row>
     <row r="9" spans="1:11" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A9" s="69" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="48"/>
+      <c r="A9" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A10" s="33"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="34"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="35"/>
     </row>
     <row r="11" spans="1:11" ht="19.5" thickBot="1">
       <c r="A11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
       <c r="H11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="37" t="s">
+      <c r="J11" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="38"/>
+      <c r="K11" s="75"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="9">
         <v>1</v>
       </c>
-      <c r="B12" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="24">
-        <v>1</v>
-      </c>
-      <c r="J12" s="35"/>
-      <c r="K12" s="36"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="73"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
         <v>2</v>
       </c>
-      <c r="B13" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="25">
-        <v>1</v>
-      </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="36"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="73"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="10">
         <v>3</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="25"/>
       <c r="I14" s="26"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="30"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="38"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="10">
         <v>4</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
       <c r="H15" s="25"/>
       <c r="I15" s="26"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="38"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="10">
         <v>5</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="25"/>
       <c r="I16" s="26"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="30"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="10">
         <v>6</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="25"/>
       <c r="I17" s="26"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="30"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="38"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="10">
         <v>7</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
       <c r="H18" s="25"/>
       <c r="I18" s="26"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="30"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="38"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="10">
         <v>8</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
       <c r="H19" s="25"/>
       <c r="I19" s="26"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="30"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="38"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="10">
         <v>9</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
       <c r="H20" s="25"/>
       <c r="I20" s="26"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="30"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="38"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="10">
         <v>10</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
       <c r="H21" s="25"/>
       <c r="I21" s="26"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="30"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="38"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="10">
         <v>11</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
       <c r="H22" s="25"/>
       <c r="I22" s="26"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="30"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="38"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="10">
         <v>12</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="2"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="32"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="28"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="10">
         <v>13</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="2"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="32"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="28"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="10">
         <v>14</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="2"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="32"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="28"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="10">
         <v>15</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
       <c r="H26" s="2"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="32"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="28"/>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="10">
         <v>16</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="2"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="32"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="28"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="10">
         <v>17</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
       <c r="H28" s="2"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="32"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="28"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="10">
         <v>18</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="2"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="32"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="28"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="10">
         <v>19</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
       <c r="H30" s="2"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="32"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="28"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="10">
         <v>20</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
       <c r="H31" s="2"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="32"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="28"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="10">
         <v>21</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
       <c r="H32" s="2"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="32"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="28"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="10">
         <v>22</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
       <c r="H33" s="2"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="32"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="28"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="10">
         <v>23</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
       <c r="H34" s="2"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="32"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="28"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="10">
         <v>24</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
       <c r="H35" s="2"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="32"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="28"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="10">
         <v>25</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
       <c r="H36" s="2"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="32"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="28"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="10">
         <v>26</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
       <c r="H37" s="2"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="32"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="28"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="10">
         <v>27</v>
       </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
       <c r="H38" s="2"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="32"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="28"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="10">
         <v>28</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
       <c r="H39" s="2"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="32"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="28"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="10">
         <v>29</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
       <c r="H40" s="2"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="32"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="28"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1">
       <c r="A41" s="11">
         <v>30</v>
       </c>
-      <c r="B41" s="72"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
-      <c r="F41" s="72"/>
-      <c r="G41" s="72"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
       <c r="H41" s="18"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="72"/>
-      <c r="K41" s="73"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="36"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" thickBot="1">
       <c r="A42" s="19"/>
@@ -2126,40 +2076,36 @@
       <c r="K42" s="21"/>
     </row>
     <row r="43" spans="1:13" s="7" customFormat="1" ht="16.149999999999999" customHeight="1">
-      <c r="A43" s="74" t="s">
+      <c r="A43" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="75"/>
-      <c r="C43" s="75"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="75"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="75"/>
-      <c r="H43" s="75"/>
-      <c r="I43" s="75"/>
-      <c r="J43" s="75"/>
-      <c r="K43" s="76"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="33"/>
     </row>
     <row r="44" spans="1:13" ht="25.15" customHeight="1">
       <c r="A44" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B44" s="22"/>
-      <c r="C44" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
       <c r="F44" s="22"/>
       <c r="G44" s="23" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="23"/>
-      <c r="I44" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="J44" s="28"/>
-      <c r="K44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="35"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
@@ -2191,11 +2137,9 @@
         <v>8</v>
       </c>
       <c r="H46" s="22"/>
-      <c r="I46" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="J46" s="28"/>
-      <c r="K46" s="34"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="35"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
@@ -2219,19 +2163,17 @@
         <v>7</v>
       </c>
       <c r="B48" s="23"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
       <c r="F48" s="23"/>
       <c r="G48" s="22" t="s">
         <v>10</v>
       </c>
       <c r="H48" s="22"/>
-      <c r="I48" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="J48" s="28"/>
-      <c r="K48" s="34"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="35"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
@@ -2250,16 +2192,58 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G8:K9"/>
+    <mergeCell ref="A1:K3"/>
+    <mergeCell ref="A4:K5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J41:K41"/>
     <mergeCell ref="B41:G41"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B19:G19"/>
@@ -2276,58 +2260,16 @@
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B24:G24"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="G8:K9"/>
-    <mergeCell ref="A1:K3"/>
-    <mergeCell ref="A4:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="J38:K38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>

</xml_diff>